<commit_message>
committed the process 5th and update 3rd and 4th
</commit_message>
<xml_diff>
--- a/data/process_03/inputData.xlsx
+++ b/data/process_03/inputData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="P_03" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
         <v>101215</v>
       </c>
       <c r="H2" s="1">
-        <v>44239</v>
+        <v>44245</v>
       </c>
       <c r="I2" s="1">
         <v>44561</v>

</xml_diff>

<commit_message>
committed changes code 18Feb2021
</commit_message>
<xml_diff>
--- a/data/process_03/inputData.xlsx
+++ b/data/process_03/inputData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Document Type</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Document Type2</t>
+  </si>
+  <si>
+    <t>Unit OfMeasure</t>
+  </si>
+  <si>
+    <t>lb</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -420,7 +426,7 @@
     <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1">
+    <row r="1" spans="1:18" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,8 +478,11 @@
       <c r="Q1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -496,7 +505,7 @@
         <v>101215</v>
       </c>
       <c r="H2" s="1">
-        <v>44245</v>
+        <v>44247</v>
       </c>
       <c r="I2" s="1">
         <v>44561</v>
@@ -524,6 +533,9 @@
       </c>
       <c r="Q2">
         <v>1272</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committed the cust ref and text from input
</commit_message>
<xml_diff>
--- a/data/process_03/inputData.xlsx
+++ b/data/process_03/inputData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Document Type</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Pricing Unit</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -429,7 +435,7 @@
     <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,8 +493,11 @@
       <c r="S1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -545,6 +554,9 @@
       </c>
       <c r="S2">
         <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
process 5 has been changed
</commit_message>
<xml_diff>
--- a/data/process_03/inputData.xlsx
+++ b/data/process_03/inputData.xlsx
@@ -420,7 +420,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -520,7 +520,7 @@
         <v>101215</v>
       </c>
       <c r="H2" s="1">
-        <v>44245</v>
+        <v>44249</v>
       </c>
       <c r="I2" s="1">
         <v>44561</v>

</xml_diff>